<commit_message>
Updated spreadsheet by OtherBarry
</commit_message>
<xml_diff>
--- a/Source/StockParts.xlsx
+++ b/Source/StockParts.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="26835" windowHeight="12585"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="28740" windowHeight="7425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks" sheetId="3" r:id="rId1"/>
@@ -22,12 +22,17 @@
     <definedName name="subs">#REF!</definedName>
     <definedName name="thresh">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
   <si>
     <t>dia</t>
   </si>
@@ -296,9 +301,6 @@
     <t>force/dia</t>
   </si>
   <si>
-    <t>force/dia^2</t>
-  </si>
-  <si>
     <t>&lt;- I agree this is a very weird formula, but it does keep true to stock.</t>
   </si>
   <si>
@@ -306,13 +308,67 @@
   </si>
   <si>
     <t>As you can see, no real agreement in any of the force ratios above.</t>
+  </si>
+  <si>
+    <t>noseCone</t>
+  </si>
+  <si>
+    <t>stability</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>rocketNoseCone</t>
+  </si>
+  <si>
+    <t>standardNoseCone</t>
+  </si>
+  <si>
+    <t>advAerodynamics</t>
+  </si>
+  <si>
+    <t>noseConeAdapter</t>
+  </si>
+  <si>
+    <t>adapterSmallMiniShort</t>
+  </si>
+  <si>
+    <t>specializedConstruction</t>
+  </si>
+  <si>
+    <t>adapterSmallMiniTall</t>
+  </si>
+  <si>
+    <t>largeAdapter</t>
+  </si>
+  <si>
+    <t>largeAdapter2</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>force/area</t>
+  </si>
+  <si>
+    <t>area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +380,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -346,17 +418,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -651,11 +731,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
@@ -663,15 +743,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="1"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:26">
       <c r="B2" t="s">
@@ -727,7 +807,7 @@
       </c>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E3" t="s">
@@ -809,15 +889,15 @@
         <v>65.4615488213486</v>
       </c>
       <c r="V4">
-        <f>SUM(E4:F4)/D4</f>
+        <f t="shared" ref="V4:V13" si="0">SUM(E4:F4)/D4</f>
         <v>849</v>
       </c>
       <c r="W4">
-        <f>E4/D4</f>
+        <f t="shared" ref="W4:W13" si="1">E4/D4</f>
         <v>382.33333333333337</v>
       </c>
       <c r="X4">
-        <f>F4/D4</f>
+        <f t="shared" ref="X4:X13" si="2">F4/D4</f>
         <v>466.66666666666669</v>
       </c>
       <c r="Z4">
@@ -842,19 +922,19 @@
         <v>24</v>
       </c>
       <c r="V5">
-        <f>SUM(E5:F5)/D5</f>
+        <f t="shared" si="0"/>
         <v>887.99999999999989</v>
       </c>
       <c r="W5">
-        <f>E5/D5</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="X5">
-        <f>F5/D5</f>
+        <f t="shared" si="2"/>
         <v>487.99999999999994</v>
       </c>
       <c r="Z5">
-        <f t="shared" ref="Z5:Z32" si="0">L5/D5</f>
+        <f t="shared" ref="Z5:Z32" si="3">L5/D5</f>
         <v>0</v>
       </c>
     </row>
@@ -902,35 +982,35 @@
         <v>2900</v>
       </c>
       <c r="R6">
-        <f>C6*PI()*B6^2*0.25</f>
+        <f t="shared" ref="R6:R13" si="4">C6*PI()*B6^2*0.25</f>
         <v>0.95873799242852575</v>
       </c>
       <c r="S6">
-        <f>D6/$R6</f>
+        <f t="shared" ref="S6:U13" si="5">D6/$R6</f>
         <v>6.518986469044033E-2</v>
       </c>
       <c r="T6">
-        <f>E6/$R6</f>
+        <f t="shared" si="5"/>
         <v>46.936702577117039</v>
       </c>
       <c r="U6">
-        <f>F6/$R6</f>
+        <f t="shared" si="5"/>
         <v>57.367080927587487</v>
       </c>
       <c r="V6">
-        <f>SUM(E6:F6)/D6</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W6">
-        <f>E6/D6</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X6">
-        <f>F6/D6</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>800</v>
       </c>
     </row>
@@ -978,35 +1058,35 @@
         <v>2900</v>
       </c>
       <c r="R7">
-        <f>C7*PI()*B7^2*0.25</f>
+        <f t="shared" si="4"/>
         <v>1.3627885319576036</v>
       </c>
       <c r="S7">
-        <f>D7/$R7</f>
+        <f t="shared" si="5"/>
         <v>9.1723695253321039E-2</v>
       </c>
       <c r="T7">
-        <f>E7/$R7</f>
+        <f t="shared" si="5"/>
         <v>66.041060582391154</v>
       </c>
       <c r="U7">
-        <f>F7/$R7</f>
+        <f t="shared" si="5"/>
         <v>80.716851822922521</v>
       </c>
       <c r="V7">
-        <f>SUM(E7:F7)/D7</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W7">
-        <f>E7/D7</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X7">
-        <f>F7/D7</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
@@ -1054,35 +1134,35 @@
         <v>2900</v>
       </c>
       <c r="R8">
-        <f>C8*PI()*B8^2*0.25</f>
+        <f t="shared" si="4"/>
         <v>2.304885900799146</v>
       </c>
       <c r="S8">
-        <f>D8/$R8</f>
+        <f t="shared" si="5"/>
         <v>0.10846523895752082</v>
       </c>
       <c r="T8">
-        <f>E8/$R8</f>
+        <f t="shared" si="5"/>
         <v>78.094972049414991</v>
       </c>
       <c r="U8">
-        <f>F8/$R8</f>
+        <f t="shared" si="5"/>
         <v>95.449410282618317</v>
       </c>
       <c r="V8">
-        <f>SUM(E8:F8)/D8</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W8">
-        <f>E8/D8</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X8">
-        <f>F8/D8</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
     </row>
@@ -1130,35 +1210,35 @@
         <v>2900</v>
       </c>
       <c r="R9">
-        <f>C9*PI()*B9^2*0.25</f>
+        <f t="shared" si="4"/>
         <v>4.6019423636569234</v>
       </c>
       <c r="S9">
-        <f>D9/$R9</f>
+        <f t="shared" si="5"/>
         <v>0.10864977448406722</v>
       </c>
       <c r="T9">
-        <f>E9/$R9</f>
+        <f t="shared" si="5"/>
         <v>78.227837628528405</v>
       </c>
       <c r="U9">
-        <f>F9/$R9</f>
+        <f t="shared" si="5"/>
         <v>95.611801545979162</v>
       </c>
       <c r="V9">
-        <f>SUM(E9:F9)/D9</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W9">
-        <f>E9/D9</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X9">
-        <f>F9/D9</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -1185,35 +1265,35 @@
         <v>23</v>
       </c>
       <c r="R10">
-        <f>C10*PI()*B10^2*0.25</f>
+        <f t="shared" si="4"/>
         <v>4.6019423636569234</v>
       </c>
       <c r="S10">
-        <f>D10/$R10</f>
+        <f t="shared" si="5"/>
         <v>0.10864977448406722</v>
       </c>
       <c r="T10">
-        <f>E10/$R10</f>
+        <f t="shared" si="5"/>
         <v>78.227837628528405</v>
       </c>
       <c r="U10">
-        <f>F10/$R10</f>
+        <f t="shared" si="5"/>
         <v>95.611801545979162</v>
       </c>
       <c r="V10">
-        <f>SUM(E10:F10)/D10</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W10">
-        <f>E10/D10</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X10">
-        <f>F10/D10</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1261,35 +1341,35 @@
         <v>2900</v>
       </c>
       <c r="R11">
-        <f>C11*PI()*B11^2*0.25</f>
+        <f t="shared" si="4"/>
         <v>9.2038847273138469</v>
       </c>
       <c r="S11">
-        <f>D11/$R11</f>
+        <f t="shared" si="5"/>
         <v>0.10864977448406722</v>
       </c>
       <c r="T11">
-        <f>E11/$R11</f>
+        <f t="shared" si="5"/>
         <v>78.227837628528405</v>
       </c>
       <c r="U11">
-        <f>F11/$R11</f>
+        <f t="shared" si="5"/>
         <v>95.611801545979162</v>
       </c>
       <c r="V11">
-        <f>SUM(E11:F11)/D11</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W11">
-        <f>E11/D11</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X11">
-        <f>F11/D11</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
     </row>
@@ -1337,35 +1417,35 @@
         <v>2900</v>
       </c>
       <c r="R12">
-        <f>C12*PI()*B12^2*0.25</f>
+        <f t="shared" si="4"/>
         <v>18.407769454627694</v>
       </c>
       <c r="S12">
-        <f>D12/$R12</f>
+        <f t="shared" si="5"/>
         <v>0.10864977448406722</v>
       </c>
       <c r="T12">
-        <f>E12/$R12</f>
+        <f t="shared" si="5"/>
         <v>78.227837628528405</v>
       </c>
       <c r="U12">
-        <f>F12/$R12</f>
+        <f t="shared" si="5"/>
         <v>95.611801545979162</v>
       </c>
       <c r="V12">
-        <f>SUM(E12:F12)/D12</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W12">
-        <f>E12/D12</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X12">
-        <f>F12/D12</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -1413,40 +1493,40 @@
         <v>2900</v>
       </c>
       <c r="R13">
-        <f>C13*PI()*B13^2*0.25</f>
+        <f t="shared" si="4"/>
         <v>36.815538909255388</v>
       </c>
       <c r="S13">
-        <f>D13/$R13</f>
+        <f t="shared" si="5"/>
         <v>0.10864977448406722</v>
       </c>
       <c r="T13">
-        <f>E13/$R13</f>
+        <f t="shared" si="5"/>
         <v>78.227837628528405</v>
       </c>
       <c r="U13">
-        <f>F13/$R13</f>
+        <f t="shared" si="5"/>
         <v>95.611801545979162</v>
       </c>
       <c r="V13">
-        <f>SUM(E13:F13)/D13</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="W13">
-        <f>E13/D13</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="X13">
-        <f>F13/D13</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E15" t="s">
@@ -1496,11 +1576,11 @@
         <v>0.70023817685104117</v>
       </c>
       <c r="S16">
-        <f>D16/$R16</f>
+        <f t="shared" ref="S16:T18" si="6">D16/$R16</f>
         <v>0.21421282780460124</v>
       </c>
       <c r="T16">
-        <f>E16/$R16</f>
+        <f t="shared" si="6"/>
         <v>142.80855186973417</v>
       </c>
       <c r="V16">
@@ -1508,7 +1588,7 @@
         <v>666.66666666666674</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1551,11 +1631,11 @@
         <v>4.908738521234052</v>
       </c>
       <c r="S17">
-        <f>D17/$R17</f>
+        <f t="shared" si="6"/>
         <v>8.148733086305042E-2</v>
       </c>
       <c r="T17">
-        <f>E17/$R17</f>
+        <f t="shared" si="6"/>
         <v>152.78874536821951</v>
       </c>
       <c r="V17">
@@ -1563,7 +1643,7 @@
         <v>1875</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1612,11 +1692,11 @@
         <v>0.11504855909142309</v>
       </c>
       <c r="S18">
-        <f>D18/$R18</f>
+        <f t="shared" si="6"/>
         <v>0.43459909793626889</v>
       </c>
       <c r="T18">
-        <f>E18/$R18</f>
+        <f t="shared" si="6"/>
         <v>434.59909793626889</v>
       </c>
       <c r="V18">
@@ -1624,7 +1704,7 @@
         <v>1000</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
     </row>
@@ -1661,7 +1741,7 @@
         <v>533.33333333333337</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1695,12 +1775,12 @@
         <v>1000</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E22" t="s">
@@ -1746,7 +1826,7 @@
         <v>428.57142857142861</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1768,7 +1848,7 @@
         <v>800</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1790,7 +1870,7 @@
         <v>800</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1812,7 +1892,7 @@
         <v>800</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1834,12 +1914,12 @@
         <v>800</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E29" t="s">
@@ -1894,19 +1974,19 @@
         <v>3600</v>
       </c>
       <c r="R30">
-        <f t="shared" ref="R30" si="1">C30*PI()*B30^2*0.25</f>
+        <f>C30*PI()*B30^2*0.25</f>
         <v>2.9452431127404308</v>
       </c>
       <c r="S30">
-        <f t="shared" ref="S30" si="2">D30/$R30</f>
+        <f t="shared" ref="S30:T32" si="7">D30/$R30</f>
         <v>0.16976527263135505</v>
       </c>
       <c r="T30">
-        <f t="shared" ref="T30" si="3">E30/$R30</f>
+        <f t="shared" si="7"/>
         <v>147.01672609875348</v>
       </c>
       <c r="V30">
-        <f t="shared" ref="V30:V32" si="4">SUM(E30:F30)/D30</f>
+        <f>SUM(E30:F30)/D30</f>
         <v>866</v>
       </c>
       <c r="Y30">
@@ -1914,7 +1994,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1959,27 +2039,27 @@
         <v>3900</v>
       </c>
       <c r="R31">
-        <f t="shared" ref="R31" si="5">C31*PI()*B31^2*0.25</f>
+        <f>C31*PI()*B31^2*0.25</f>
         <v>8.7130108751904416</v>
       </c>
       <c r="S31">
-        <f t="shared" ref="S31" si="6">D31/$R31</f>
+        <f t="shared" si="7"/>
         <v>0.17215633280926146</v>
       </c>
       <c r="T31">
-        <f t="shared" ref="T31" si="7">E31/$R31</f>
+        <f t="shared" si="7"/>
         <v>97.555255258581482</v>
       </c>
       <c r="V31">
-        <f t="shared" si="4"/>
+        <f>SUM(E31:F31)/D31</f>
         <v>566.66666666666663</v>
       </c>
       <c r="Y31">
-        <f t="shared" ref="Y31:Y32" si="8">O31/N31</f>
+        <f>O31/N31</f>
         <v>1.2698412698412698</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2024,27 +2104,27 @@
         <v>3600</v>
       </c>
       <c r="R32">
-        <f t="shared" ref="R32" si="9">C32*PI()*B32^2*0.25</f>
+        <f>C32*PI()*B32^2*0.25</f>
         <v>8.8357293382212935E-3</v>
       </c>
       <c r="S32">
-        <f t="shared" ref="S32" si="10">D32/$R32</f>
+        <f t="shared" si="7"/>
         <v>1.4147106052612919</v>
       </c>
       <c r="T32">
-        <f t="shared" ref="T32" si="11">E32/$R32</f>
+        <f t="shared" si="7"/>
         <v>905.41478736722684</v>
       </c>
       <c r="V32">
-        <f t="shared" si="4"/>
+        <f>SUM(E32:F32)/D32</f>
         <v>640</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="8"/>
+        <f>O32/N32</f>
         <v>30.555555555555557</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2054,21 +2134,25 @@
     <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:N15"/>
+  <dimension ref="A4:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:17">
       <c r="B4" t="s">
         <v>59</v>
       </c>
@@ -2076,31 +2160,34 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>68</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>87</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>88</v>
       </c>
-      <c r="N4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="P4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2112,36 +2199,44 @@
         <v>1.25</v>
       </c>
       <c r="D5">
+        <f>PI() * (C5/2)^2</f>
+        <v>1.227184630308513</v>
+      </c>
+      <c r="E5">
         <v>250</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.05</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I10" si="0">2*PI()*(C5/2)*B5</f>
+      <c r="J5">
+        <f t="shared" ref="J5:J10" si="0">2*PI()*(C5/2)*B5</f>
         <v>0.77772717953554549</v>
       </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J10" si="1">E5/I5</f>
+      <c r="K5">
+        <f t="shared" ref="K5:K10" si="1">F5/J5</f>
         <v>6.4289896657411069E-2</v>
       </c>
-      <c r="L5">
-        <f>D5/I5</f>
+      <c r="N5">
+        <f>E5/J5</f>
         <v>321.44948328705533</v>
       </c>
-      <c r="M5">
-        <f>D5/C5</f>
+      <c r="O5">
+        <f>E5/C5</f>
         <v>200</v>
       </c>
-      <c r="N5">
-        <f>D5/C5^2</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="P5">
+        <f>E5/D5</f>
+        <v>203.71832715762602</v>
+      </c>
+      <c r="Q5">
+        <f>P5*PI()</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -2153,36 +2248,44 @@
         <v>0.625</v>
       </c>
       <c r="D6">
+        <f t="shared" ref="D6:D13" si="2">PI() * (C6/2)^2</f>
+        <v>0.30679615757712825</v>
+      </c>
+      <c r="E6">
         <v>15</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>0.29809763729805244</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>5.031908382756578E-2</v>
       </c>
-      <c r="L6">
-        <f t="shared" ref="L6:L7" si="2">D6/I6</f>
+      <c r="N6">
+        <f>E6/J6</f>
         <v>50.319083827565777</v>
       </c>
-      <c r="M6">
-        <f t="shared" ref="M6:M11" si="3">D6/C6</f>
+      <c r="O6">
+        <f t="shared" ref="O6:O11" si="3">E6/C6</f>
         <v>24</v>
       </c>
-      <c r="N6">
-        <f t="shared" ref="N6:N11" si="4">D6/C6^2</f>
-        <v>38.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="P6">
+        <f t="shared" ref="P6:P11" si="4">E6/D6</f>
+        <v>48.892398517830244</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q11" si="5">P6*PI()</f>
+        <v>153.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -2194,36 +2297,44 @@
         <v>2.5</v>
       </c>
       <c r="D7">
+        <f t="shared" si="2"/>
+        <v>4.908738521234052</v>
+      </c>
+      <c r="E7">
         <v>250</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>6.4114180507156515</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>6.2388694175908782E-2</v>
       </c>
-      <c r="L7">
-        <f>D7/I7</f>
+      <c r="N7">
+        <f>E7/J7</f>
         <v>38.992933859942987</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>50.929581789406505</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2234,36 +2345,44 @@
         <v>2.5</v>
       </c>
       <c r="D9">
+        <f t="shared" si="2"/>
+        <v>4.908738521234052</v>
+      </c>
+      <c r="E9">
         <v>600</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.45</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>65</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>1.5707963267948966</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>0.28647889756541162</v>
       </c>
-      <c r="L9">
-        <f t="shared" ref="L8:L11" si="5">D9/I9</f>
+      <c r="N9">
+        <f>E9/J9</f>
         <v>381.9718634205488</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <f t="shared" si="4"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>122.23099629457562</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2275,36 +2394,44 @@
         <v>1.25</v>
       </c>
       <c r="D10">
+        <f t="shared" si="2"/>
+        <v>1.227184630308513</v>
+      </c>
+      <c r="E10">
         <v>250</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>65</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>1.4396850989899801</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>5.2094725473380746E-2</v>
       </c>
-      <c r="L10">
-        <f t="shared" si="5"/>
+      <c r="N10">
+        <f>E10/J10</f>
         <v>173.64908491126917</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <f t="shared" si="4"/>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>203.71832715762602</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -2316,137 +2443,165 @@
         <v>0.625</v>
       </c>
       <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0.30679615757712825</v>
+      </c>
+      <c r="E11">
         <v>15</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.02</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>65</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f>2*PI()*(C11/2)*B11</f>
         <v>0.29809763729805244</v>
       </c>
-      <c r="J11">
-        <f>E11/I11</f>
+      <c r="K11">
+        <f>F11/J11</f>
         <v>6.7092111770087712E-2</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="5"/>
+      <c r="N11">
+        <f>E11/J11</f>
         <v>50.319083827565777</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <f t="shared" si="4"/>
-        <v>38.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>48.892398517830244</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>153.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>86</v>
       </c>
       <c r="C13">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <f>ROUND((((C13-0.625)/0.625*(14-8)+8)*C13)^2/5, 0)*5</f>
-        <v>265</v>
-      </c>
-      <c r="E13" t="s">
+        <f t="shared" si="2"/>
+        <v>12.566370614359172</v>
+      </c>
+      <c r="E13">
+        <f>ROUND(IF(D13&lt;D11, 25,
+IF(D13&lt;D10, (D13-D11)/(D10-D11)*(300-25)+25,
+IF(C13&lt;C9,  (D13-D10)/(D9-D10)*(800-300)+300,
+ D13/D9*800)))/5, 0)*5</f>
+        <v>2050</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="F14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="E14" t="s">
+    <row r="15" spans="1:17">
+      <c r="F15" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="E15" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:18">
+      <c r="B1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>47</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>51</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>54</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>55</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>52</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>53</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>69</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2454,50 +2609,496 @@
         <v>1.25</v>
       </c>
       <c r="C3">
+        <v>1.25</v>
+      </c>
+      <c r="D3">
         <f>0.75*2*1.25</f>
         <v>1.875</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.3</v>
       </c>
-      <c r="G3">
-        <v>0.2</v>
-      </c>
       <c r="H3">
+        <v>0.2</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>70</v>
-      </c>
-      <c r="J3">
-        <v>50</v>
       </c>
       <c r="K3">
         <v>50</v>
       </c>
-      <c r="N3">
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="O3">
         <v>3000</v>
       </c>
-      <c r="P3">
-        <f>C3*PI()*B3^2*0.25</f>
+      <c r="Q3">
+        <f>D3*PI()*B3^2*0.25</f>
         <v>2.3009711818284617</v>
       </c>
-      <c r="Q3">
-        <f>D3/$P3</f>
+      <c r="R3">
+        <f>E3/$Q3</f>
         <v>0.17383963917450757</v>
       </c>
     </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5">
+        <v>1.25</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="E5">
+        <v>0.03</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>0.5</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" t="s">
+        <v>94</v>
+      </c>
+      <c r="O5">
+        <v>3400</v>
+      </c>
+      <c r="Q5">
+        <f>((((B5/2)^2)+((B5/2)*(C5/2))+((C5/2)^2))*D5*3.14159265)/3</f>
+        <v>0.23111977177734375</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R13" si="0">E5/$Q5</f>
+        <v>0.12980282807176449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2.0950000000000002</v>
+      </c>
+      <c r="E6">
+        <v>0.4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" t="s">
+        <v>94</v>
+      </c>
+      <c r="O6">
+        <v>3400</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q13" si="1">((((B6/2)^2)+((B6/2)*(C6/2))+((C6/2)^2))*D6*3.14159265)/3</f>
+        <v>3.4279357300781257</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>0.11668830208519798</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7">
+        <v>0.625</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>0.25</v>
+      </c>
+      <c r="J7">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7">
+        <v>3400</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>4.2440135083007813E-2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>2.356260172226408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9">
+        <v>1.25</v>
+      </c>
+      <c r="C9">
+        <v>0.625</v>
+      </c>
+      <c r="D9">
+        <v>0.995</v>
+      </c>
+      <c r="E9">
+        <v>0.3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>0.1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L9" t="s">
+        <v>94</v>
+      </c>
+      <c r="O9">
+        <v>3400</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>0.71227841169433592</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>0.42118362016107358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10">
+        <v>1.25</v>
+      </c>
+      <c r="C10">
+        <v>0.625</v>
+      </c>
+      <c r="D10">
+        <v>0.1875</v>
+      </c>
+      <c r="E10">
+        <v>0.04</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="H10">
+        <v>0.2</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>50</v>
+      </c>
+      <c r="O10">
+        <v>2900</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>0.13422331878662111</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>0.29801081035396848</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11">
+        <v>1.25</v>
+      </c>
+      <c r="C11">
+        <v>0.625</v>
+      </c>
+      <c r="D11">
+        <v>0.6875</v>
+      </c>
+      <c r="E11">
+        <v>0.05</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11">
+        <v>0.2</v>
+      </c>
+      <c r="I11">
+        <v>0.2</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>2900</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>0.49215216888427737</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>0.10159459443885291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <v>2.5</v>
+      </c>
+      <c r="C12">
+        <v>1.25</v>
+      </c>
+      <c r="D12">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>0.2</v>
+      </c>
+      <c r="H12">
+        <v>0.3</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>200</v>
+      </c>
+      <c r="L12">
+        <v>200</v>
+      </c>
+      <c r="O12">
+        <v>2900</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>3.5936056549804682</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>2.7827204652076248E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>2.5</v>
+      </c>
+      <c r="C13">
+        <v>1.25</v>
+      </c>
+      <c r="D13">
+        <v>0.3785</v>
+      </c>
+      <c r="E13">
+        <v>0.08</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13">
+        <v>0.3</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>200</v>
+      </c>
+      <c r="L13">
+        <v>200</v>
+      </c>
+      <c r="O13">
+        <v>2900</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>1.0838085580957031</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>7.381377403087068E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:O15" si="2">SUM(E3:E13)/9</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>1.161111111111111</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>19.333333333333332</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>61.111111111111114</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>61.111111111111114</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>3133.3333333333335</v>
+      </c>
+      <c r="Q15">
+        <f>SUM(Q3:Q13)/9</f>
+        <v>1.3353927701342605</v>
+      </c>
+      <c r="R15">
+        <f>SUM(R3:R13)/9</f>
+        <v>0.41100232724385782</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:K1"/>
+  <mergeCells count="3">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tech changes for ARM
</commit_message>
<xml_diff>
--- a/Source/StockParts.xlsx
+++ b/Source/StockParts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="4080" windowWidth="30840" windowHeight="18980"/>
+    <workbookView xWindow="3765" yWindow="4080" windowWidth="30840" windowHeight="18975"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="subs">#REF!</definedName>
     <definedName name="thresh">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="146">
   <si>
     <t>dia</t>
   </si>
@@ -498,13 +498,19 @@
   </si>
   <si>
     <t>Size3to2Adapter</t>
+  </si>
+  <si>
+    <t>fuelTank1-2</t>
+  </si>
+  <si>
+    <t>fuelTank3-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,10 +633,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -948,32 +954,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.5" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="N1" s="5" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="5"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:28">
       <c r="B2" t="s">
@@ -1593,6 +1599,9 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>144</v>
+      </c>
       <c r="C12">
         <v>2.5</v>
       </c>
@@ -1609,7 +1618,7 @@
         <v>1760</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J12">
         <v>0.2</v>
@@ -1666,6 +1675,9 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
       <c r="C13">
         <v>2.5</v>
       </c>
@@ -1682,7 +1694,7 @@
         <v>3520</v>
       </c>
       <c r="I13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13">
         <v>0.2</v>
@@ -3093,14 +3105,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" t="s">
@@ -3399,36 +3411,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" t="s">
@@ -3938,10 +3950,10 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>3.75</v>
       </c>
       <c r="C17">

</xml_diff>